<commit_message>
adding module docstring. add option to open different sheets. file formatting.
</commit_message>
<xml_diff>
--- a/Sustain/Mock_Data.xlsx
+++ b/Sustain/Mock_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yello\Documents\GitHub\SheCodes\Sustain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9755E2-1B34-4E78-A9D1-6A81234EB733}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A091151C-0BA8-4A4D-97E6-46815EE2B9AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -510,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -690,8 +690,17 @@
       <c r="N4" s="2">
         <v>5</v>
       </c>
-      <c r="R4" s="2">
+      <c r="O4" s="2">
         <v>6</v>
+      </c>
+      <c r="P4" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>7</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -726,8 +735,17 @@
       <c r="N5" s="2">
         <v>5</v>
       </c>
-      <c r="R5" s="2">
+      <c r="O5" s="2">
         <v>6</v>
+      </c>
+      <c r="P5" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>7</v>
+      </c>
+      <c r="R5" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -762,8 +780,17 @@
       <c r="N6" s="2">
         <v>5</v>
       </c>
-      <c r="R6" s="2">
-        <v>5</v>
+      <c r="O6" s="2">
+        <v>5</v>
+      </c>
+      <c r="P6" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>6</v>
+      </c>
+      <c r="R6" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -798,8 +825,17 @@
       <c r="N7" s="2">
         <v>5</v>
       </c>
-      <c r="R7" s="2">
-        <v>5</v>
+      <c r="O7" s="2">
+        <v>5</v>
+      </c>
+      <c r="P7" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>6</v>
+      </c>
+      <c r="R7" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -834,8 +870,17 @@
       <c r="N8" s="2">
         <v>4</v>
       </c>
-      <c r="R8" s="2">
-        <v>4</v>
+      <c r="O8" s="2">
+        <v>4</v>
+      </c>
+      <c r="P8" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>5</v>
+      </c>
+      <c r="R8" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -870,8 +915,17 @@
       <c r="N9" s="2">
         <v>5</v>
       </c>
-      <c r="R9" s="2">
+      <c r="O9" s="2">
         <v>6</v>
+      </c>
+      <c r="P9" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>6</v>
+      </c>
+      <c r="R9" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -915,7 +969,7 @@
       <c r="Q10" s="2">
         <v>12</v>
       </c>
-      <c r="R10" s="2">
+      <c r="R10" s="1">
         <v>12</v>
       </c>
     </row>
@@ -951,8 +1005,17 @@
       <c r="N11" s="2">
         <v>5</v>
       </c>
-      <c r="R11" s="2">
+      <c r="O11" s="2">
         <v>6</v>
+      </c>
+      <c r="P11" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>6</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
@@ -963,27 +1026,13 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2">
-        <v>2</v>
-      </c>
-      <c r="J12" s="2">
-        <v>2</v>
-      </c>
-      <c r="K12" s="2">
-        <v>3</v>
-      </c>
-      <c r="L12" s="2">
-        <v>3</v>
-      </c>
-      <c r="M12" s="2">
-        <v>4</v>
-      </c>
-      <c r="N12" s="2">
-        <v>4</v>
-      </c>
-      <c r="R12" s="2">
-        <v>5</v>
-      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
@@ -1009,27 +1058,13 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2">
-        <v>2</v>
-      </c>
-      <c r="J14" s="2">
-        <v>3</v>
-      </c>
-      <c r="K14" s="2">
-        <v>4</v>
-      </c>
-      <c r="L14" s="2">
-        <v>6</v>
-      </c>
-      <c r="M14" s="2">
-        <v>7</v>
-      </c>
-      <c r="N14" s="2">
-        <v>8</v>
-      </c>
-      <c r="R14" s="2">
-        <v>9</v>
-      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
@@ -1039,27 +1074,13 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2">
-        <v>2</v>
-      </c>
-      <c r="J15" s="2">
-        <v>2</v>
-      </c>
-      <c r="K15" s="2">
-        <v>3</v>
-      </c>
-      <c r="L15" s="2">
-        <v>3</v>
-      </c>
-      <c r="M15" s="2">
-        <v>4</v>
-      </c>
-      <c r="N15" s="2">
-        <v>4</v>
-      </c>
-      <c r="R15" s="2">
-        <v>5</v>
-      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
@@ -1085,27 +1106,13 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="2">
-        <v>2</v>
-      </c>
-      <c r="J17" s="2">
-        <v>2</v>
-      </c>
-      <c r="K17" s="2">
-        <v>2</v>
-      </c>
-      <c r="L17" s="2">
-        <v>3</v>
-      </c>
-      <c r="M17" s="2">
-        <v>3</v>
-      </c>
-      <c r="N17" s="2">
-        <v>3</v>
-      </c>
-      <c r="R17" s="2">
-        <v>4</v>
-      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="R17" s="2"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
@@ -1115,27 +1122,13 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="2">
-        <v>2</v>
-      </c>
-      <c r="J18" s="2">
-        <v>2</v>
-      </c>
-      <c r="K18" s="2">
-        <v>3</v>
-      </c>
-      <c r="L18" s="2">
-        <v>3</v>
-      </c>
-      <c r="M18" s="2">
-        <v>4</v>
-      </c>
-      <c r="N18" s="2">
-        <v>5</v>
-      </c>
-      <c r="R18" s="2">
-        <v>6</v>
-      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="R18" s="2"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
@@ -1161,27 +1154,13 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="2">
-        <v>2</v>
-      </c>
-      <c r="J20" s="2">
-        <v>2</v>
-      </c>
-      <c r="K20" s="2">
-        <v>3</v>
-      </c>
-      <c r="L20" s="2">
-        <v>3</v>
-      </c>
-      <c r="M20" s="2">
-        <v>4</v>
-      </c>
-      <c r="N20" s="2">
-        <v>4</v>
-      </c>
-      <c r="R20" s="2">
-        <v>4</v>
-      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="R20" s="2"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
@@ -1191,27 +1170,13 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="2">
-        <v>2</v>
-      </c>
-      <c r="J21" s="2">
-        <v>2</v>
-      </c>
-      <c r="K21" s="2">
-        <v>3</v>
-      </c>
-      <c r="L21" s="2">
-        <v>3</v>
-      </c>
-      <c r="M21" s="2">
-        <v>4</v>
-      </c>
-      <c r="N21" s="2">
-        <v>5</v>
-      </c>
-      <c r="R21" s="2">
-        <v>6</v>
-      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="R21" s="2"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B22" s="2"/>
@@ -1221,27 +1186,13 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="2">
-        <v>2</v>
-      </c>
-      <c r="J22" s="2">
-        <v>2</v>
-      </c>
-      <c r="K22" s="2">
-        <v>3</v>
-      </c>
-      <c r="L22" s="2">
-        <v>3</v>
-      </c>
-      <c r="M22" s="2">
-        <v>4</v>
-      </c>
-      <c r="N22" s="2">
-        <v>4</v>
-      </c>
-      <c r="R22" s="2">
-        <v>5</v>
-      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="R22" s="2"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B23" s="2"/>
@@ -1251,27 +1202,13 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="2">
-        <v>2</v>
-      </c>
-      <c r="J23" s="2">
-        <v>2</v>
-      </c>
-      <c r="K23" s="2">
-        <v>3</v>
-      </c>
-      <c r="L23" s="2">
-        <v>3</v>
-      </c>
-      <c r="M23" s="2">
-        <v>3</v>
-      </c>
-      <c r="N23" s="2">
-        <v>4</v>
-      </c>
-      <c r="R23" s="2">
-        <v>4</v>
-      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="R23" s="2"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B24" s="2"/>
@@ -1281,36 +1218,16 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="2">
-        <v>8</v>
-      </c>
-      <c r="J24" s="2">
-        <v>9</v>
-      </c>
-      <c r="K24" s="2">
-        <v>10</v>
-      </c>
-      <c r="L24" s="2">
-        <v>11</v>
-      </c>
-      <c r="M24" s="2">
-        <v>12</v>
-      </c>
-      <c r="N24" s="2">
-        <v>12</v>
-      </c>
-      <c r="O24" s="2">
-        <v>12</v>
-      </c>
-      <c r="P24" s="2">
-        <v>13</v>
-      </c>
-      <c r="Q24" s="2">
-        <v>13</v>
-      </c>
-      <c r="R24" s="2">
-        <v>13</v>
-      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R25">
@@ -1325,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DC5A709-A7BD-4744-A8DD-88697AE92691}">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F13"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -1464,7 +1381,7 @@
         <v>8</v>
       </c>
       <c r="R3" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="28" x14ac:dyDescent="0.35">
@@ -1536,27 +1453,13 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2">
-        <v>2</v>
-      </c>
-      <c r="M6" s="2">
-        <v>2</v>
-      </c>
-      <c r="N6" s="2">
-        <v>2</v>
-      </c>
-      <c r="O6" s="2">
-        <v>3</v>
-      </c>
-      <c r="P6" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>3</v>
-      </c>
-      <c r="R6" s="2">
-        <v>4</v>
-      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
@@ -1569,27 +1472,13 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2">
-        <v>2</v>
-      </c>
-      <c r="M7" s="2">
-        <v>2</v>
-      </c>
-      <c r="N7" s="2">
-        <v>3</v>
-      </c>
-      <c r="O7" s="2">
-        <v>3</v>
-      </c>
-      <c r="P7" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>5</v>
-      </c>
-      <c r="R7" s="2">
-        <v>6</v>
-      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B8" s="2"/>
@@ -1621,27 +1510,13 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2">
-        <v>2</v>
-      </c>
-      <c r="M9" s="2">
-        <v>2</v>
-      </c>
-      <c r="N9" s="2">
-        <v>3</v>
-      </c>
-      <c r="O9" s="2">
-        <v>3</v>
-      </c>
-      <c r="P9" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>4</v>
-      </c>
-      <c r="R9" s="2">
-        <v>4</v>
-      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
@@ -1654,27 +1529,13 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2">
-        <v>2</v>
-      </c>
-      <c r="M10" s="2">
-        <v>2</v>
-      </c>
-      <c r="N10" s="2">
-        <v>3</v>
-      </c>
-      <c r="O10" s="2">
-        <v>3</v>
-      </c>
-      <c r="P10" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>5</v>
-      </c>
-      <c r="R10" s="2">
-        <v>6</v>
-      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
@@ -1687,27 +1548,13 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="2">
-        <v>2</v>
-      </c>
-      <c r="M11" s="2">
-        <v>2</v>
-      </c>
-      <c r="N11" s="2">
-        <v>3</v>
-      </c>
-      <c r="O11" s="2">
-        <v>3</v>
-      </c>
-      <c r="P11" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>4</v>
-      </c>
-      <c r="R11" s="2">
-        <v>5</v>
-      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B12" s="2"/>
@@ -1720,27 +1567,13 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="2">
-        <v>2</v>
-      </c>
-      <c r="M12" s="2">
-        <v>2</v>
-      </c>
-      <c r="N12" s="2">
-        <v>3</v>
-      </c>
-      <c r="O12" s="2">
-        <v>3</v>
-      </c>
-      <c r="P12" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>4</v>
-      </c>
-      <c r="R12" s="2">
-        <v>4</v>
-      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
@@ -1750,36 +1583,16 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2">
-        <v>8</v>
-      </c>
-      <c r="J13" s="2">
-        <v>9</v>
-      </c>
-      <c r="K13" s="2">
-        <v>10</v>
-      </c>
-      <c r="L13" s="2">
-        <v>11</v>
-      </c>
-      <c r="M13" s="2">
-        <v>12</v>
-      </c>
-      <c r="N13" s="2">
-        <v>12</v>
-      </c>
-      <c r="O13" s="2">
-        <v>12</v>
-      </c>
-      <c r="P13" s="2">
-        <v>13</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>13</v>
-      </c>
-      <c r="R13" s="2">
-        <v>13</v>
-      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R13">
@@ -1794,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DA778F-0970-40D8-864B-3890B384B0D9}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -1933,7 +1746,7 @@
         <v>3</v>
       </c>
       <c r="R3" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -1976,17 +1789,11 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -2001,205 +1808,99 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2">
-        <v>2</v>
-      </c>
-      <c r="M6" s="2">
-        <v>2</v>
-      </c>
-      <c r="N6" s="2">
-        <v>3</v>
-      </c>
-      <c r="O6" s="2">
-        <v>3</v>
-      </c>
-      <c r="P6" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>4</v>
-      </c>
-      <c r="R6" s="2">
-        <v>4</v>
-      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2">
-        <v>2</v>
-      </c>
-      <c r="M7" s="2">
-        <v>2</v>
-      </c>
-      <c r="N7" s="2">
-        <v>3</v>
-      </c>
-      <c r="O7" s="2">
-        <v>3</v>
-      </c>
-      <c r="P7" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>5</v>
-      </c>
-      <c r="R7" s="2">
-        <v>6</v>
-      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2">
-        <v>2</v>
-      </c>
-      <c r="M8" s="2">
-        <v>2</v>
-      </c>
-      <c r="N8" s="2">
-        <v>3</v>
-      </c>
-      <c r="O8" s="2">
-        <v>3</v>
-      </c>
-      <c r="P8" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>4</v>
-      </c>
-      <c r="R8" s="2">
-        <v>5</v>
-      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2">
-        <v>2</v>
-      </c>
-      <c r="M9" s="2">
-        <v>2</v>
-      </c>
-      <c r="N9" s="2">
-        <v>3</v>
-      </c>
-      <c r="O9" s="2">
-        <v>3</v>
-      </c>
-      <c r="P9" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>4</v>
-      </c>
-      <c r="R9" s="2">
-        <v>4</v>
-      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2">
-        <v>8</v>
-      </c>
-      <c r="J10" s="2">
-        <v>9</v>
-      </c>
-      <c r="K10" s="2">
-        <v>10</v>
-      </c>
-      <c r="L10" s="2">
-        <v>11</v>
-      </c>
-      <c r="M10" s="2">
-        <v>12</v>
-      </c>
-      <c r="N10" s="2">
-        <v>12</v>
-      </c>
-      <c r="O10" s="2">
-        <v>12</v>
-      </c>
-      <c r="P10" s="2">
-        <v>13</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>13</v>
-      </c>
-      <c r="R10" s="2">
-        <v>13</v>
-      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2211,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7E4A37-A077-40A5-92F2-A4034C820DCF}">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -2328,29 +2029,35 @@
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>3</v>
+      </c>
       <c r="L3" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M3" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N3" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O3" s="2">
-        <v>3</v>
-      </c>
-      <c r="P3" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>4</v>
-      </c>
-      <c r="R3" s="2">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="P3" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>5</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -2367,29 +2074,35 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="I4" s="2">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>3</v>
+      </c>
       <c r="L4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M4" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N4" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O4" s="2">
-        <v>3</v>
-      </c>
-      <c r="P4" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>5</v>
-      </c>
-      <c r="R4" s="2">
         <v>6</v>
+      </c>
+      <c r="P4" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>8</v>
+      </c>
+      <c r="R4" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -2406,29 +2119,35 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>3</v>
+      </c>
       <c r="L5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M5" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O5" s="2">
-        <v>3</v>
-      </c>
-      <c r="P5" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>4</v>
-      </c>
-      <c r="R5" s="2">
-        <v>5</v>
+        <v>5</v>
+      </c>
+      <c r="P5" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>5</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -2445,29 +2164,35 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>3</v>
+      </c>
       <c r="L6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N6" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O6" s="2">
-        <v>3</v>
-      </c>
-      <c r="P6" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>4</v>
-      </c>
-      <c r="R6" s="2">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="P6" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>5</v>
+      </c>
+      <c r="R6" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>